<commit_message>
a bunch of weekend changes
</commit_message>
<xml_diff>
--- a/templates/cpr1000/cin_cover.xlsx
+++ b/templates/cpr1000/cin_cover.xlsx
@@ -516,10 +516,6 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>${issuer}</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>${unit}</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
@@ -537,6 +533,10 @@
   </si>
   <si>
     <t>${date}</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>${supplyerCode}</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -1130,119 +1130,17 @@
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1250,23 +1148,19 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="7" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="7" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -1280,6 +1174,42 @@
       <alignment horizontal="left" vertical="top" wrapText="1"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -1325,6 +1255,9 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1348,67 +1281,134 @@
       <alignment horizontal="left" vertical="top" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="14" fontId="7" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="7" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="5">
@@ -2651,7 +2651,7 @@
   <dimension ref="A1:AB34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A14" sqref="A14:M14"/>
+      <selection activeCell="B10" sqref="B10:T10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.15"/>
@@ -2660,530 +2660,530 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:28" x14ac:dyDescent="0.15">
-      <c r="A1" s="19"/>
-      <c r="B1" s="20"/>
-      <c r="C1" s="20"/>
-      <c r="D1" s="20"/>
-      <c r="E1" s="20"/>
-      <c r="F1" s="20"/>
-      <c r="G1" s="20"/>
-      <c r="H1" s="20"/>
-      <c r="I1" s="20"/>
-      <c r="J1" s="20"/>
-      <c r="K1" s="20"/>
-      <c r="L1" s="20"/>
-      <c r="M1" s="20"/>
-      <c r="N1" s="20"/>
-      <c r="O1" s="20"/>
-      <c r="P1" s="20"/>
-      <c r="Q1" s="20"/>
-      <c r="R1" s="20"/>
-      <c r="S1" s="20"/>
-      <c r="T1" s="20"/>
-      <c r="U1" s="20"/>
-      <c r="V1" s="20"/>
-      <c r="W1" s="20"/>
-      <c r="X1" s="20"/>
-      <c r="Y1" s="20"/>
-      <c r="Z1" s="20"/>
-      <c r="AA1" s="20"/>
-      <c r="AB1" s="21"/>
+      <c r="A1" s="88"/>
+      <c r="B1" s="89"/>
+      <c r="C1" s="89"/>
+      <c r="D1" s="89"/>
+      <c r="E1" s="89"/>
+      <c r="F1" s="89"/>
+      <c r="G1" s="89"/>
+      <c r="H1" s="89"/>
+      <c r="I1" s="89"/>
+      <c r="J1" s="89"/>
+      <c r="K1" s="89"/>
+      <c r="L1" s="89"/>
+      <c r="M1" s="89"/>
+      <c r="N1" s="89"/>
+      <c r="O1" s="89"/>
+      <c r="P1" s="89"/>
+      <c r="Q1" s="89"/>
+      <c r="R1" s="89"/>
+      <c r="S1" s="89"/>
+      <c r="T1" s="89"/>
+      <c r="U1" s="89"/>
+      <c r="V1" s="89"/>
+      <c r="W1" s="89"/>
+      <c r="X1" s="89"/>
+      <c r="Y1" s="89"/>
+      <c r="Z1" s="89"/>
+      <c r="AA1" s="89"/>
+      <c r="AB1" s="90"/>
     </row>
     <row r="2" spans="1:28" ht="16" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="22"/>
-      <c r="B2" s="23"/>
-      <c r="C2" s="23"/>
-      <c r="D2" s="23"/>
-      <c r="E2" s="23"/>
-      <c r="F2" s="23"/>
-      <c r="G2" s="23"/>
-      <c r="H2" s="23"/>
-      <c r="I2" s="23"/>
-      <c r="J2" s="23"/>
-      <c r="K2" s="23"/>
-      <c r="L2" s="23"/>
-      <c r="M2" s="23"/>
-      <c r="N2" s="23"/>
-      <c r="O2" s="23"/>
-      <c r="P2" s="23"/>
-      <c r="Q2" s="23"/>
-      <c r="R2" s="23"/>
-      <c r="S2" s="23"/>
-      <c r="T2" s="23"/>
-      <c r="U2" s="23"/>
-      <c r="V2" s="23"/>
-      <c r="W2" s="23"/>
-      <c r="X2" s="23"/>
-      <c r="Y2" s="23"/>
-      <c r="Z2" s="23"/>
-      <c r="AA2" s="23"/>
-      <c r="AB2" s="24"/>
+      <c r="A2" s="91"/>
+      <c r="B2" s="92"/>
+      <c r="C2" s="92"/>
+      <c r="D2" s="92"/>
+      <c r="E2" s="92"/>
+      <c r="F2" s="92"/>
+      <c r="G2" s="92"/>
+      <c r="H2" s="92"/>
+      <c r="I2" s="92"/>
+      <c r="J2" s="92"/>
+      <c r="K2" s="92"/>
+      <c r="L2" s="92"/>
+      <c r="M2" s="92"/>
+      <c r="N2" s="92"/>
+      <c r="O2" s="92"/>
+      <c r="P2" s="92"/>
+      <c r="Q2" s="92"/>
+      <c r="R2" s="92"/>
+      <c r="S2" s="92"/>
+      <c r="T2" s="92"/>
+      <c r="U2" s="92"/>
+      <c r="V2" s="92"/>
+      <c r="W2" s="92"/>
+      <c r="X2" s="92"/>
+      <c r="Y2" s="92"/>
+      <c r="Z2" s="92"/>
+      <c r="AA2" s="92"/>
+      <c r="AB2" s="93"/>
     </row>
     <row r="3" spans="1:28" ht="20" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="25" t="s">
+      <c r="A3" s="94" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="26"/>
-      <c r="C3" s="26"/>
-      <c r="D3" s="26"/>
-      <c r="E3" s="26"/>
-      <c r="F3" s="26"/>
-      <c r="G3" s="26"/>
-      <c r="H3" s="26"/>
-      <c r="I3" s="26"/>
-      <c r="J3" s="26"/>
-      <c r="K3" s="26"/>
-      <c r="L3" s="26"/>
-      <c r="M3" s="26"/>
-      <c r="N3" s="26"/>
-      <c r="O3" s="26"/>
-      <c r="P3" s="26"/>
-      <c r="Q3" s="26"/>
-      <c r="R3" s="26"/>
-      <c r="S3" s="26"/>
-      <c r="T3" s="26"/>
-      <c r="U3" s="26"/>
-      <c r="V3" s="26"/>
-      <c r="W3" s="26"/>
-      <c r="X3" s="26"/>
-      <c r="Y3" s="26"/>
-      <c r="Z3" s="26"/>
-      <c r="AA3" s="26"/>
-      <c r="AB3" s="27"/>
+      <c r="B3" s="95"/>
+      <c r="C3" s="95"/>
+      <c r="D3" s="95"/>
+      <c r="E3" s="95"/>
+      <c r="F3" s="95"/>
+      <c r="G3" s="95"/>
+      <c r="H3" s="95"/>
+      <c r="I3" s="95"/>
+      <c r="J3" s="95"/>
+      <c r="K3" s="95"/>
+      <c r="L3" s="95"/>
+      <c r="M3" s="95"/>
+      <c r="N3" s="95"/>
+      <c r="O3" s="95"/>
+      <c r="P3" s="95"/>
+      <c r="Q3" s="95"/>
+      <c r="R3" s="95"/>
+      <c r="S3" s="95"/>
+      <c r="T3" s="95"/>
+      <c r="U3" s="95"/>
+      <c r="V3" s="95"/>
+      <c r="W3" s="95"/>
+      <c r="X3" s="95"/>
+      <c r="Y3" s="95"/>
+      <c r="Z3" s="95"/>
+      <c r="AA3" s="95"/>
+      <c r="AB3" s="96"/>
     </row>
     <row r="4" spans="1:28" ht="23" x14ac:dyDescent="0.15">
-      <c r="A4" s="28" t="s">
+      <c r="A4" s="97" t="s">
         <v>54</v>
       </c>
-      <c r="B4" s="29"/>
-      <c r="C4" s="29"/>
-      <c r="D4" s="29"/>
-      <c r="E4" s="29"/>
-      <c r="F4" s="29"/>
-      <c r="G4" s="29"/>
-      <c r="H4" s="29"/>
-      <c r="I4" s="29"/>
-      <c r="J4" s="29"/>
-      <c r="K4" s="29"/>
-      <c r="L4" s="29"/>
-      <c r="M4" s="29"/>
-      <c r="N4" s="29"/>
-      <c r="O4" s="29"/>
-      <c r="P4" s="30" t="s">
+      <c r="B4" s="98"/>
+      <c r="C4" s="98"/>
+      <c r="D4" s="98"/>
+      <c r="E4" s="98"/>
+      <c r="F4" s="98"/>
+      <c r="G4" s="98"/>
+      <c r="H4" s="98"/>
+      <c r="I4" s="98"/>
+      <c r="J4" s="98"/>
+      <c r="K4" s="98"/>
+      <c r="L4" s="98"/>
+      <c r="M4" s="98"/>
+      <c r="N4" s="98"/>
+      <c r="O4" s="98"/>
+      <c r="P4" s="99" t="s">
         <v>1</v>
       </c>
-      <c r="Q4" s="30"/>
-      <c r="R4" s="30"/>
-      <c r="S4" s="30"/>
-      <c r="T4" s="30"/>
-      <c r="U4" s="30"/>
-      <c r="V4" s="30"/>
-      <c r="W4" s="30"/>
-      <c r="X4" s="30"/>
-      <c r="Y4" s="30"/>
-      <c r="Z4" s="30"/>
-      <c r="AA4" s="30"/>
-      <c r="AB4" s="31"/>
+      <c r="Q4" s="99"/>
+      <c r="R4" s="99"/>
+      <c r="S4" s="99"/>
+      <c r="T4" s="99"/>
+      <c r="U4" s="99"/>
+      <c r="V4" s="99"/>
+      <c r="W4" s="99"/>
+      <c r="X4" s="99"/>
+      <c r="Y4" s="99"/>
+      <c r="Z4" s="99"/>
+      <c r="AA4" s="99"/>
+      <c r="AB4" s="100"/>
     </row>
     <row r="5" spans="1:28" ht="16" x14ac:dyDescent="0.15">
-      <c r="A5" s="32" t="s">
+      <c r="A5" s="101" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="33"/>
-      <c r="C5" s="33"/>
-      <c r="D5" s="33"/>
-      <c r="E5" s="33"/>
-      <c r="F5" s="33"/>
-      <c r="G5" s="33"/>
-      <c r="H5" s="33"/>
-      <c r="I5" s="33"/>
-      <c r="J5" s="33"/>
-      <c r="K5" s="33"/>
-      <c r="L5" s="33"/>
-      <c r="M5" s="33"/>
-      <c r="N5" s="33"/>
-      <c r="O5" s="33"/>
-      <c r="P5" s="33"/>
-      <c r="Q5" s="33"/>
-      <c r="R5" s="33"/>
-      <c r="S5" s="33"/>
-      <c r="T5" s="33"/>
-      <c r="U5" s="33"/>
-      <c r="V5" s="33"/>
-      <c r="W5" s="33"/>
-      <c r="X5" s="33"/>
-      <c r="Y5" s="33"/>
-      <c r="Z5" s="33"/>
-      <c r="AA5" s="33"/>
-      <c r="AB5" s="34"/>
+      <c r="B5" s="102"/>
+      <c r="C5" s="102"/>
+      <c r="D5" s="102"/>
+      <c r="E5" s="102"/>
+      <c r="F5" s="102"/>
+      <c r="G5" s="102"/>
+      <c r="H5" s="102"/>
+      <c r="I5" s="102"/>
+      <c r="J5" s="102"/>
+      <c r="K5" s="102"/>
+      <c r="L5" s="102"/>
+      <c r="M5" s="102"/>
+      <c r="N5" s="102"/>
+      <c r="O5" s="102"/>
+      <c r="P5" s="102"/>
+      <c r="Q5" s="102"/>
+      <c r="R5" s="102"/>
+      <c r="S5" s="102"/>
+      <c r="T5" s="102"/>
+      <c r="U5" s="102"/>
+      <c r="V5" s="102"/>
+      <c r="W5" s="102"/>
+      <c r="X5" s="102"/>
+      <c r="Y5" s="102"/>
+      <c r="Z5" s="102"/>
+      <c r="AA5" s="102"/>
+      <c r="AB5" s="103"/>
     </row>
     <row r="6" spans="1:28" ht="19" x14ac:dyDescent="0.15">
-      <c r="A6" s="15" t="s">
+      <c r="A6" s="84" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="16"/>
-      <c r="C6" s="16"/>
-      <c r="D6" s="16"/>
-      <c r="E6" s="16"/>
-      <c r="F6" s="16"/>
-      <c r="G6" s="16"/>
-      <c r="H6" s="16"/>
-      <c r="I6" s="16"/>
-      <c r="J6" s="16"/>
-      <c r="K6" s="16"/>
-      <c r="L6" s="16"/>
-      <c r="M6" s="16"/>
-      <c r="N6" s="16"/>
-      <c r="O6" s="16"/>
-      <c r="P6" s="16"/>
-      <c r="Q6" s="16"/>
-      <c r="R6" s="16"/>
-      <c r="S6" s="16"/>
-      <c r="T6" s="16"/>
-      <c r="U6" s="16"/>
-      <c r="V6" s="16"/>
-      <c r="W6" s="17" t="str">
+      <c r="B6" s="85"/>
+      <c r="C6" s="85"/>
+      <c r="D6" s="85"/>
+      <c r="E6" s="85"/>
+      <c r="F6" s="85"/>
+      <c r="G6" s="85"/>
+      <c r="H6" s="85"/>
+      <c r="I6" s="85"/>
+      <c r="J6" s="85"/>
+      <c r="K6" s="85"/>
+      <c r="L6" s="85"/>
+      <c r="M6" s="85"/>
+      <c r="N6" s="85"/>
+      <c r="O6" s="85"/>
+      <c r="P6" s="85"/>
+      <c r="Q6" s="85"/>
+      <c r="R6" s="85"/>
+      <c r="S6" s="85"/>
+      <c r="T6" s="85"/>
+      <c r="U6" s="85"/>
+      <c r="V6" s="85"/>
+      <c r="W6" s="86" t="str">
         <f>IF(AD3="HYH3","(C)",)&amp;IF(AD3="HYH4","(C)",)&amp;IF(AD3="YJ1","(D)",)&amp;IF(AD3="YJ2","(D)",)&amp;IF(AD3="ND3","(E)",)&amp;IF(AD3="ND4","(E)",)&amp;IF(AD3="FCG1","(FCG)",)&amp;IF(AD3="FCG2","(FCG)",)&amp;IF(AD3="YJ3","(YJ34)",)&amp;IF(AD3="YJ4","(YJ34)",)</f>
         <v/>
       </c>
-      <c r="X6" s="17"/>
-      <c r="Y6" s="17"/>
-      <c r="Z6" s="17"/>
-      <c r="AA6" s="17"/>
-      <c r="AB6" s="18"/>
+      <c r="X6" s="86"/>
+      <c r="Y6" s="86"/>
+      <c r="Z6" s="86"/>
+      <c r="AA6" s="86"/>
+      <c r="AB6" s="87"/>
     </row>
     <row r="7" spans="1:28" ht="19" x14ac:dyDescent="0.15">
-      <c r="A7" s="35" t="s">
-        <v>60</v>
-      </c>
-      <c r="B7" s="36"/>
-      <c r="C7" s="36"/>
-      <c r="D7" s="36"/>
-      <c r="E7" s="36"/>
-      <c r="F7" s="36"/>
-      <c r="G7" s="36"/>
-      <c r="H7" s="36"/>
-      <c r="I7" s="36"/>
-      <c r="J7" s="36"/>
-      <c r="K7" s="36"/>
-      <c r="L7" s="36"/>
-      <c r="M7" s="36"/>
-      <c r="N7" s="36"/>
-      <c r="O7" s="36"/>
-      <c r="P7" s="36"/>
-      <c r="Q7" s="36"/>
-      <c r="R7" s="36"/>
-      <c r="S7" s="36"/>
-      <c r="T7" s="36"/>
-      <c r="U7" s="36"/>
-      <c r="V7" s="36"/>
-      <c r="W7" s="36"/>
-      <c r="X7" s="36"/>
-      <c r="Y7" s="36"/>
-      <c r="Z7" s="36"/>
+      <c r="A7" s="70" t="s">
+        <v>59</v>
+      </c>
+      <c r="B7" s="71"/>
+      <c r="C7" s="71"/>
+      <c r="D7" s="71"/>
+      <c r="E7" s="71"/>
+      <c r="F7" s="71"/>
+      <c r="G7" s="71"/>
+      <c r="H7" s="71"/>
+      <c r="I7" s="71"/>
+      <c r="J7" s="71"/>
+      <c r="K7" s="71"/>
+      <c r="L7" s="71"/>
+      <c r="M7" s="71"/>
+      <c r="N7" s="71"/>
+      <c r="O7" s="71"/>
+      <c r="P7" s="71"/>
+      <c r="Q7" s="71"/>
+      <c r="R7" s="71"/>
+      <c r="S7" s="71"/>
+      <c r="T7" s="71"/>
+      <c r="U7" s="71"/>
+      <c r="V7" s="71"/>
+      <c r="W7" s="71"/>
+      <c r="X7" s="71"/>
+      <c r="Y7" s="71"/>
+      <c r="Z7" s="71"/>
       <c r="AA7" s="1"/>
       <c r="AB7" s="2"/>
     </row>
     <row r="8" spans="1:28" x14ac:dyDescent="0.15">
-      <c r="A8" s="37" t="s">
+      <c r="A8" s="72" t="s">
         <v>4</v>
       </c>
-      <c r="B8" s="38" t="s">
+      <c r="B8" s="73" t="s">
         <v>5</v>
       </c>
-      <c r="C8" s="38"/>
-      <c r="D8" s="38"/>
-      <c r="E8" s="38"/>
-      <c r="F8" s="38"/>
-      <c r="G8" s="38"/>
-      <c r="H8" s="38"/>
-      <c r="I8" s="38"/>
-      <c r="J8" s="38"/>
-      <c r="K8" s="38"/>
-      <c r="L8" s="38"/>
-      <c r="M8" s="38"/>
-      <c r="N8" s="38"/>
-      <c r="O8" s="38"/>
-      <c r="P8" s="38"/>
-      <c r="Q8" s="38"/>
-      <c r="R8" s="38"/>
-      <c r="S8" s="38"/>
-      <c r="T8" s="39"/>
-      <c r="U8" s="40" t="s">
+      <c r="C8" s="73"/>
+      <c r="D8" s="73"/>
+      <c r="E8" s="73"/>
+      <c r="F8" s="73"/>
+      <c r="G8" s="73"/>
+      <c r="H8" s="73"/>
+      <c r="I8" s="73"/>
+      <c r="J8" s="73"/>
+      <c r="K8" s="73"/>
+      <c r="L8" s="73"/>
+      <c r="M8" s="73"/>
+      <c r="N8" s="73"/>
+      <c r="O8" s="73"/>
+      <c r="P8" s="73"/>
+      <c r="Q8" s="73"/>
+      <c r="R8" s="73"/>
+      <c r="S8" s="73"/>
+      <c r="T8" s="74"/>
+      <c r="U8" s="75" t="s">
         <v>6</v>
       </c>
-      <c r="V8" s="41"/>
-      <c r="W8" s="42"/>
-      <c r="X8" s="40" t="s">
+      <c r="V8" s="76"/>
+      <c r="W8" s="77"/>
+      <c r="X8" s="75" t="s">
         <v>7</v>
       </c>
-      <c r="Y8" s="41"/>
-      <c r="Z8" s="41"/>
-      <c r="AA8" s="41"/>
-      <c r="AB8" s="46"/>
+      <c r="Y8" s="76"/>
+      <c r="Z8" s="76"/>
+      <c r="AA8" s="76"/>
+      <c r="AB8" s="81"/>
     </row>
     <row r="9" spans="1:28" x14ac:dyDescent="0.15">
-      <c r="A9" s="37"/>
+      <c r="A9" s="72"/>
       <c r="B9" s="3"/>
-      <c r="C9" s="48" t="s">
+      <c r="C9" s="83" t="s">
         <v>55</v>
       </c>
-      <c r="D9" s="48"/>
+      <c r="D9" s="83"/>
       <c r="E9" s="4"/>
-      <c r="F9" s="48" t="s">
+      <c r="F9" s="83" t="s">
         <v>8</v>
       </c>
-      <c r="G9" s="48"/>
-      <c r="H9" s="48"/>
+      <c r="G9" s="83"/>
+      <c r="H9" s="83"/>
       <c r="I9" s="5"/>
-      <c r="J9" s="48" t="s">
-        <v>56</v>
-      </c>
-      <c r="K9" s="48"/>
-      <c r="L9" s="48"/>
-      <c r="M9" s="48"/>
+      <c r="J9" s="83" t="s">
+        <v>61</v>
+      </c>
+      <c r="K9" s="83"/>
+      <c r="L9" s="83"/>
+      <c r="M9" s="83"/>
       <c r="N9" s="5"/>
       <c r="O9" s="5" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="P9" s="4"/>
-      <c r="Q9" s="48" t="s">
+      <c r="Q9" s="83" t="s">
         <v>9</v>
       </c>
-      <c r="R9" s="48"/>
-      <c r="S9" s="48"/>
+      <c r="R9" s="83"/>
+      <c r="S9" s="83"/>
       <c r="T9" s="3"/>
-      <c r="U9" s="43"/>
-      <c r="V9" s="44"/>
-      <c r="W9" s="45"/>
-      <c r="X9" s="43"/>
-      <c r="Y9" s="44"/>
-      <c r="Z9" s="44"/>
-      <c r="AA9" s="44"/>
-      <c r="AB9" s="47"/>
+      <c r="U9" s="78"/>
+      <c r="V9" s="79"/>
+      <c r="W9" s="80"/>
+      <c r="X9" s="78"/>
+      <c r="Y9" s="79"/>
+      <c r="Z9" s="79"/>
+      <c r="AA9" s="79"/>
+      <c r="AB9" s="82"/>
     </row>
     <row r="10" spans="1:28" x14ac:dyDescent="0.15">
       <c r="A10" s="7" t="s">
         <v>53</v>
       </c>
-      <c r="B10" s="49" t="s">
+      <c r="B10" s="69" t="s">
         <v>10</v>
       </c>
-      <c r="C10" s="49"/>
-      <c r="D10" s="49"/>
-      <c r="E10" s="49"/>
-      <c r="F10" s="49"/>
-      <c r="G10" s="49"/>
-      <c r="H10" s="49"/>
-      <c r="I10" s="49"/>
-      <c r="J10" s="49"/>
-      <c r="K10" s="49"/>
-      <c r="L10" s="49"/>
-      <c r="M10" s="49"/>
-      <c r="N10" s="49"/>
-      <c r="O10" s="49"/>
-      <c r="P10" s="49"/>
-      <c r="Q10" s="49"/>
-      <c r="R10" s="49"/>
-      <c r="S10" s="49"/>
-      <c r="T10" s="49"/>
+      <c r="C10" s="69"/>
+      <c r="D10" s="69"/>
+      <c r="E10" s="69"/>
+      <c r="F10" s="69"/>
+      <c r="G10" s="69"/>
+      <c r="H10" s="69"/>
+      <c r="I10" s="69"/>
+      <c r="J10" s="69"/>
+      <c r="K10" s="69"/>
+      <c r="L10" s="69"/>
+      <c r="M10" s="69"/>
+      <c r="N10" s="69"/>
+      <c r="O10" s="69"/>
+      <c r="P10" s="69"/>
+      <c r="Q10" s="69"/>
+      <c r="R10" s="69"/>
+      <c r="S10" s="69"/>
+      <c r="T10" s="69"/>
       <c r="U10" s="6"/>
-      <c r="V10" s="50" t="s">
+      <c r="V10" s="66" t="s">
         <v>11</v>
       </c>
-      <c r="W10" s="51"/>
+      <c r="W10" s="68"/>
       <c r="X10" s="6"/>
-      <c r="Y10" s="50" t="s">
+      <c r="Y10" s="66" t="s">
         <v>12</v>
       </c>
-      <c r="Z10" s="50"/>
-      <c r="AA10" s="50"/>
-      <c r="AB10" s="52"/>
+      <c r="Z10" s="66"/>
+      <c r="AA10" s="66"/>
+      <c r="AB10" s="67"/>
     </row>
     <row r="11" spans="1:28" ht="16" x14ac:dyDescent="0.15">
       <c r="A11" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="B11" s="53" t="s">
+      <c r="B11" s="19" t="s">
         <v>14</v>
       </c>
-      <c r="C11" s="54"/>
-      <c r="D11" s="54"/>
-      <c r="E11" s="54"/>
-      <c r="F11" s="54"/>
-      <c r="G11" s="54"/>
-      <c r="H11" s="54"/>
-      <c r="I11" s="54"/>
-      <c r="J11" s="54"/>
-      <c r="K11" s="54"/>
-      <c r="L11" s="55" t="s">
+      <c r="C11" s="20"/>
+      <c r="D11" s="20"/>
+      <c r="E11" s="20"/>
+      <c r="F11" s="20"/>
+      <c r="G11" s="20"/>
+      <c r="H11" s="20"/>
+      <c r="I11" s="20"/>
+      <c r="J11" s="20"/>
+      <c r="K11" s="20"/>
+      <c r="L11" s="63" t="s">
         <v>15</v>
       </c>
-      <c r="M11" s="55"/>
-      <c r="N11" s="55"/>
-      <c r="O11" s="55"/>
-      <c r="P11" s="55"/>
-      <c r="Q11" s="55"/>
-      <c r="R11" s="55"/>
-      <c r="S11" s="55"/>
-      <c r="T11" s="56"/>
+      <c r="M11" s="63"/>
+      <c r="N11" s="63"/>
+      <c r="O11" s="63"/>
+      <c r="P11" s="63"/>
+      <c r="Q11" s="63"/>
+      <c r="R11" s="63"/>
+      <c r="S11" s="63"/>
+      <c r="T11" s="53"/>
       <c r="U11" s="6"/>
-      <c r="V11" s="50" t="s">
+      <c r="V11" s="66" t="s">
         <v>16</v>
       </c>
-      <c r="W11" s="51"/>
+      <c r="W11" s="68"/>
       <c r="X11" s="6"/>
-      <c r="Y11" s="50" t="s">
+      <c r="Y11" s="66" t="s">
         <v>17</v>
       </c>
-      <c r="Z11" s="50"/>
-      <c r="AA11" s="50"/>
-      <c r="AB11" s="52"/>
+      <c r="Z11" s="66"/>
+      <c r="AA11" s="66"/>
+      <c r="AB11" s="67"/>
     </row>
     <row r="12" spans="1:28" ht="16" x14ac:dyDescent="0.15">
-      <c r="A12" s="57" t="s">
-        <v>61</v>
-      </c>
-      <c r="B12" s="53" t="s">
+      <c r="A12" s="61" t="s">
+        <v>60</v>
+      </c>
+      <c r="B12" s="19" t="s">
         <v>18</v>
       </c>
-      <c r="C12" s="54"/>
-      <c r="D12" s="54"/>
-      <c r="E12" s="54"/>
-      <c r="F12" s="54"/>
-      <c r="G12" s="54"/>
-      <c r="H12" s="54"/>
-      <c r="I12" s="54"/>
-      <c r="J12" s="54"/>
-      <c r="K12" s="54"/>
-      <c r="L12" s="55" t="s">
+      <c r="C12" s="20"/>
+      <c r="D12" s="20"/>
+      <c r="E12" s="20"/>
+      <c r="F12" s="20"/>
+      <c r="G12" s="20"/>
+      <c r="H12" s="20"/>
+      <c r="I12" s="20"/>
+      <c r="J12" s="20"/>
+      <c r="K12" s="20"/>
+      <c r="L12" s="63" t="s">
         <v>19</v>
       </c>
-      <c r="M12" s="55"/>
-      <c r="N12" s="55"/>
-      <c r="O12" s="55"/>
-      <c r="P12" s="55"/>
-      <c r="Q12" s="55"/>
-      <c r="R12" s="55"/>
-      <c r="S12" s="55"/>
-      <c r="T12" s="56"/>
+      <c r="M12" s="63"/>
+      <c r="N12" s="63"/>
+      <c r="O12" s="63"/>
+      <c r="P12" s="63"/>
+      <c r="Q12" s="63"/>
+      <c r="R12" s="63"/>
+      <c r="S12" s="63"/>
+      <c r="T12" s="53"/>
       <c r="U12" s="6"/>
-      <c r="V12" s="59" t="s">
+      <c r="V12" s="64" t="s">
         <v>20</v>
       </c>
-      <c r="W12" s="60"/>
+      <c r="W12" s="65"/>
       <c r="X12" s="6"/>
-      <c r="Y12" s="50" t="s">
+      <c r="Y12" s="66" t="s">
         <v>21</v>
       </c>
-      <c r="Z12" s="50"/>
-      <c r="AA12" s="50"/>
-      <c r="AB12" s="52"/>
+      <c r="Z12" s="66"/>
+      <c r="AA12" s="66"/>
+      <c r="AB12" s="67"/>
     </row>
     <row r="13" spans="1:28" ht="16" x14ac:dyDescent="0.15">
-      <c r="A13" s="58"/>
-      <c r="B13" s="53" t="s">
+      <c r="A13" s="62"/>
+      <c r="B13" s="19" t="s">
         <v>22</v>
       </c>
-      <c r="C13" s="54"/>
-      <c r="D13" s="54"/>
-      <c r="E13" s="54"/>
-      <c r="F13" s="54"/>
-      <c r="G13" s="54"/>
-      <c r="H13" s="54"/>
-      <c r="I13" s="54"/>
-      <c r="J13" s="54"/>
-      <c r="K13" s="54"/>
-      <c r="L13" s="55">
+      <c r="C13" s="20"/>
+      <c r="D13" s="20"/>
+      <c r="E13" s="20"/>
+      <c r="F13" s="20"/>
+      <c r="G13" s="20"/>
+      <c r="H13" s="20"/>
+      <c r="I13" s="20"/>
+      <c r="J13" s="20"/>
+      <c r="K13" s="20"/>
+      <c r="L13" s="63">
         <v>100</v>
       </c>
-      <c r="M13" s="55"/>
-      <c r="N13" s="55"/>
-      <c r="O13" s="55"/>
-      <c r="P13" s="55"/>
-      <c r="Q13" s="55"/>
-      <c r="R13" s="55"/>
-      <c r="S13" s="55"/>
-      <c r="T13" s="56"/>
+      <c r="M13" s="63"/>
+      <c r="N13" s="63"/>
+      <c r="O13" s="63"/>
+      <c r="P13" s="63"/>
+      <c r="Q13" s="63"/>
+      <c r="R13" s="63"/>
+      <c r="S13" s="63"/>
+      <c r="T13" s="53"/>
       <c r="U13" s="6"/>
-      <c r="V13" s="50" t="s">
+      <c r="V13" s="66" t="s">
         <v>23</v>
       </c>
-      <c r="W13" s="51"/>
+      <c r="W13" s="68"/>
       <c r="X13" s="6"/>
-      <c r="Y13" s="50" t="s">
+      <c r="Y13" s="66" t="s">
         <v>24</v>
       </c>
-      <c r="Z13" s="50"/>
-      <c r="AA13" s="50"/>
-      <c r="AB13" s="52"/>
+      <c r="Z13" s="66"/>
+      <c r="AA13" s="66"/>
+      <c r="AB13" s="67"/>
     </row>
     <row r="14" spans="1:28" x14ac:dyDescent="0.15">
-      <c r="A14" s="64" t="s">
+      <c r="A14" s="39" t="s">
         <v>25</v>
       </c>
-      <c r="B14" s="65"/>
-      <c r="C14" s="65"/>
-      <c r="D14" s="65"/>
-      <c r="E14" s="65"/>
-      <c r="F14" s="65"/>
-      <c r="G14" s="65"/>
-      <c r="H14" s="65"/>
-      <c r="I14" s="65"/>
-      <c r="J14" s="65"/>
-      <c r="K14" s="65"/>
-      <c r="L14" s="65"/>
-      <c r="M14" s="65"/>
-      <c r="N14" s="66" t="str">
+      <c r="B14" s="40"/>
+      <c r="C14" s="40"/>
+      <c r="D14" s="40"/>
+      <c r="E14" s="40"/>
+      <c r="F14" s="40"/>
+      <c r="G14" s="40"/>
+      <c r="H14" s="40"/>
+      <c r="I14" s="40"/>
+      <c r="J14" s="40"/>
+      <c r="K14" s="40"/>
+      <c r="L14" s="40"/>
+      <c r="M14" s="40"/>
+      <c r="N14" s="41" t="str">
         <f>IF(AD3="HYH3","AA357110201W00B04GN",)&amp;IF(AD3="HYH4","AA457110201W00B04GN",)&amp;IF(AD3="YJ1","PY157110620W00A04GN",)&amp;IF(AD3="YJ2","PY257110620W00A04GN",)&amp;IF(AD3="ND3","AB357110602W00B44GN",)&amp;IF(AD3="ND4","AB457110602W00B44GN",)&amp;IF(AD3="FCG1","BL157110033W00B04GN",)&amp;IF(AD3="FCG2","BL257110034W00B04GN",)&amp;IF(AD3="YJ3","PY357110033W00A04GN",)&amp;IF(AD3="YJ4","PY457110034W00A04GN",)</f>
         <v/>
       </c>
-      <c r="O14" s="67"/>
-      <c r="P14" s="67"/>
-      <c r="Q14" s="67"/>
-      <c r="R14" s="67"/>
-      <c r="S14" s="67"/>
-      <c r="T14" s="67"/>
-      <c r="U14" s="68"/>
-      <c r="V14" s="68"/>
-      <c r="W14" s="68"/>
-      <c r="X14" s="68"/>
-      <c r="Y14" s="69"/>
-      <c r="Z14" s="69"/>
-      <c r="AA14" s="69"/>
-      <c r="AB14" s="70"/>
+      <c r="O14" s="42"/>
+      <c r="P14" s="42"/>
+      <c r="Q14" s="42"/>
+      <c r="R14" s="42"/>
+      <c r="S14" s="42"/>
+      <c r="T14" s="42"/>
+      <c r="U14" s="43"/>
+      <c r="V14" s="43"/>
+      <c r="W14" s="43"/>
+      <c r="X14" s="43"/>
+      <c r="Y14" s="44"/>
+      <c r="Z14" s="44"/>
+      <c r="AA14" s="44"/>
+      <c r="AB14" s="45"/>
     </row>
     <row r="15" spans="1:28" x14ac:dyDescent="0.15">
-      <c r="A15" s="64" t="s">
+      <c r="A15" s="39" t="s">
         <v>26</v>
       </c>
-      <c r="B15" s="65"/>
-      <c r="C15" s="65"/>
-      <c r="D15" s="65"/>
-      <c r="E15" s="65"/>
-      <c r="F15" s="65"/>
-      <c r="G15" s="65"/>
-      <c r="H15" s="65"/>
-      <c r="I15" s="65"/>
-      <c r="J15" s="65"/>
-      <c r="K15" s="65"/>
-      <c r="L15" s="65"/>
-      <c r="M15" s="65"/>
-      <c r="N15" s="71" t="s">
+      <c r="B15" s="40"/>
+      <c r="C15" s="40"/>
+      <c r="D15" s="40"/>
+      <c r="E15" s="40"/>
+      <c r="F15" s="40"/>
+      <c r="G15" s="40"/>
+      <c r="H15" s="40"/>
+      <c r="I15" s="40"/>
+      <c r="J15" s="40"/>
+      <c r="K15" s="40"/>
+      <c r="L15" s="40"/>
+      <c r="M15" s="40"/>
+      <c r="N15" s="46" t="s">
         <v>27</v>
       </c>
-      <c r="O15" s="72"/>
-      <c r="P15" s="72"/>
-      <c r="Q15" s="72"/>
-      <c r="R15" s="72"/>
-      <c r="S15" s="72"/>
-      <c r="T15" s="73"/>
-      <c r="U15" s="74" t="s">
+      <c r="O15" s="47"/>
+      <c r="P15" s="47"/>
+      <c r="Q15" s="47"/>
+      <c r="R15" s="47"/>
+      <c r="S15" s="47"/>
+      <c r="T15" s="48"/>
+      <c r="U15" s="49" t="s">
         <v>28</v>
       </c>
-      <c r="V15" s="74"/>
-      <c r="W15" s="74"/>
-      <c r="X15" s="75"/>
+      <c r="V15" s="49"/>
+      <c r="W15" s="49"/>
+      <c r="X15" s="50"/>
       <c r="Y15" s="8"/>
       <c r="Z15" s="9" t="s">
         <v>29</v>
@@ -3194,36 +3194,36 @@
       </c>
     </row>
     <row r="16" spans="1:28" ht="46" x14ac:dyDescent="0.15">
-      <c r="A16" s="64" t="s">
+      <c r="A16" s="39" t="s">
         <v>31</v>
       </c>
-      <c r="B16" s="65"/>
-      <c r="C16" s="65"/>
-      <c r="D16" s="65"/>
-      <c r="E16" s="65"/>
-      <c r="F16" s="65"/>
-      <c r="G16" s="65"/>
-      <c r="H16" s="65"/>
-      <c r="I16" s="65"/>
-      <c r="J16" s="65"/>
-      <c r="K16" s="65"/>
-      <c r="L16" s="65"/>
-      <c r="M16" s="65"/>
-      <c r="N16" s="71" t="s">
+      <c r="B16" s="40"/>
+      <c r="C16" s="40"/>
+      <c r="D16" s="40"/>
+      <c r="E16" s="40"/>
+      <c r="F16" s="40"/>
+      <c r="G16" s="40"/>
+      <c r="H16" s="40"/>
+      <c r="I16" s="40"/>
+      <c r="J16" s="40"/>
+      <c r="K16" s="40"/>
+      <c r="L16" s="40"/>
+      <c r="M16" s="40"/>
+      <c r="N16" s="46" t="s">
         <v>27</v>
       </c>
-      <c r="O16" s="72"/>
-      <c r="P16" s="72"/>
-      <c r="Q16" s="72"/>
-      <c r="R16" s="72"/>
-      <c r="S16" s="72"/>
-      <c r="T16" s="73"/>
-      <c r="U16" s="74" t="s">
+      <c r="O16" s="47"/>
+      <c r="P16" s="47"/>
+      <c r="Q16" s="47"/>
+      <c r="R16" s="47"/>
+      <c r="S16" s="47"/>
+      <c r="T16" s="48"/>
+      <c r="U16" s="49" t="s">
         <v>32</v>
       </c>
-      <c r="V16" s="74"/>
-      <c r="W16" s="74"/>
-      <c r="X16" s="75"/>
+      <c r="V16" s="49"/>
+      <c r="W16" s="49"/>
+      <c r="X16" s="50"/>
       <c r="Y16" s="8"/>
       <c r="Z16" s="9" t="s">
         <v>33</v>
@@ -3234,36 +3234,36 @@
       </c>
     </row>
     <row r="17" spans="1:28" ht="28" x14ac:dyDescent="0.15">
-      <c r="A17" s="76" t="s">
+      <c r="A17" s="51" t="s">
         <v>35</v>
       </c>
-      <c r="B17" s="77"/>
-      <c r="C17" s="77"/>
-      <c r="D17" s="77"/>
-      <c r="E17" s="77"/>
-      <c r="F17" s="77"/>
-      <c r="G17" s="77"/>
-      <c r="H17" s="77"/>
-      <c r="I17" s="77"/>
-      <c r="J17" s="77"/>
-      <c r="K17" s="77"/>
-      <c r="L17" s="77"/>
-      <c r="M17" s="77"/>
-      <c r="N17" s="56" t="s">
+      <c r="B17" s="52"/>
+      <c r="C17" s="52"/>
+      <c r="D17" s="52"/>
+      <c r="E17" s="52"/>
+      <c r="F17" s="52"/>
+      <c r="G17" s="52"/>
+      <c r="H17" s="52"/>
+      <c r="I17" s="52"/>
+      <c r="J17" s="52"/>
+      <c r="K17" s="52"/>
+      <c r="L17" s="52"/>
+      <c r="M17" s="52"/>
+      <c r="N17" s="53" t="s">
         <v>36</v>
       </c>
-      <c r="O17" s="78"/>
-      <c r="P17" s="78"/>
-      <c r="Q17" s="78"/>
-      <c r="R17" s="78"/>
-      <c r="S17" s="78"/>
-      <c r="T17" s="79"/>
-      <c r="U17" s="74" t="s">
+      <c r="O17" s="54"/>
+      <c r="P17" s="54"/>
+      <c r="Q17" s="54"/>
+      <c r="R17" s="54"/>
+      <c r="S17" s="54"/>
+      <c r="T17" s="55"/>
+      <c r="U17" s="49" t="s">
         <v>37</v>
       </c>
-      <c r="V17" s="74"/>
-      <c r="W17" s="74"/>
-      <c r="X17" s="75"/>
+      <c r="V17" s="49"/>
+      <c r="W17" s="49"/>
+      <c r="X17" s="50"/>
       <c r="Y17" s="8"/>
       <c r="Z17" s="9" t="s">
         <v>38</v>
@@ -3274,63 +3274,63 @@
       </c>
     </row>
     <row r="18" spans="1:28" ht="16" x14ac:dyDescent="0.15">
-      <c r="A18" s="80" t="s">
+      <c r="A18" s="56" t="s">
         <v>40</v>
       </c>
-      <c r="B18" s="81"/>
-      <c r="C18" s="81"/>
-      <c r="D18" s="81"/>
-      <c r="E18" s="81"/>
-      <c r="F18" s="81"/>
-      <c r="G18" s="81"/>
-      <c r="H18" s="81"/>
-      <c r="I18" s="81"/>
-      <c r="J18" s="81"/>
-      <c r="K18" s="81"/>
-      <c r="L18" s="81"/>
-      <c r="M18" s="81"/>
-      <c r="N18" s="81"/>
-      <c r="O18" s="81"/>
-      <c r="P18" s="81"/>
-      <c r="Q18" s="81"/>
-      <c r="R18" s="81"/>
-      <c r="S18" s="81"/>
-      <c r="T18" s="81"/>
-      <c r="U18" s="81"/>
-      <c r="V18" s="81"/>
-      <c r="W18" s="81"/>
-      <c r="X18" s="81"/>
-      <c r="Y18" s="81"/>
-      <c r="Z18" s="81"/>
-      <c r="AA18" s="81"/>
-      <c r="AB18" s="82"/>
+      <c r="B18" s="57"/>
+      <c r="C18" s="57"/>
+      <c r="D18" s="57"/>
+      <c r="E18" s="57"/>
+      <c r="F18" s="57"/>
+      <c r="G18" s="57"/>
+      <c r="H18" s="57"/>
+      <c r="I18" s="57"/>
+      <c r="J18" s="57"/>
+      <c r="K18" s="57"/>
+      <c r="L18" s="57"/>
+      <c r="M18" s="57"/>
+      <c r="N18" s="57"/>
+      <c r="O18" s="57"/>
+      <c r="P18" s="57"/>
+      <c r="Q18" s="57"/>
+      <c r="R18" s="57"/>
+      <c r="S18" s="57"/>
+      <c r="T18" s="57"/>
+      <c r="U18" s="57"/>
+      <c r="V18" s="57"/>
+      <c r="W18" s="57"/>
+      <c r="X18" s="57"/>
+      <c r="Y18" s="57"/>
+      <c r="Z18" s="57"/>
+      <c r="AA18" s="57"/>
+      <c r="AB18" s="58"/>
     </row>
     <row r="19" spans="1:28" x14ac:dyDescent="0.15">
-      <c r="A19" s="83" t="s">
-        <v>60</v>
-      </c>
-      <c r="B19" s="84"/>
-      <c r="C19" s="84"/>
-      <c r="D19" s="84"/>
-      <c r="E19" s="84"/>
-      <c r="F19" s="84"/>
-      <c r="G19" s="84"/>
-      <c r="H19" s="84"/>
-      <c r="I19" s="84"/>
-      <c r="J19" s="84"/>
-      <c r="K19" s="84"/>
-      <c r="L19" s="84"/>
-      <c r="M19" s="84"/>
-      <c r="N19" s="84"/>
-      <c r="O19" s="84"/>
-      <c r="P19" s="84"/>
-      <c r="Q19" s="84"/>
-      <c r="R19" s="84"/>
-      <c r="S19" s="84"/>
-      <c r="T19" s="84"/>
-      <c r="U19" s="84"/>
-      <c r="V19" s="84"/>
-      <c r="W19" s="84"/>
+      <c r="A19" s="59" t="s">
+        <v>59</v>
+      </c>
+      <c r="B19" s="60"/>
+      <c r="C19" s="60"/>
+      <c r="D19" s="60"/>
+      <c r="E19" s="60"/>
+      <c r="F19" s="60"/>
+      <c r="G19" s="60"/>
+      <c r="H19" s="60"/>
+      <c r="I19" s="60"/>
+      <c r="J19" s="60"/>
+      <c r="K19" s="60"/>
+      <c r="L19" s="60"/>
+      <c r="M19" s="60"/>
+      <c r="N19" s="60"/>
+      <c r="O19" s="60"/>
+      <c r="P19" s="60"/>
+      <c r="Q19" s="60"/>
+      <c r="R19" s="60"/>
+      <c r="S19" s="60"/>
+      <c r="T19" s="60"/>
+      <c r="U19" s="60"/>
+      <c r="V19" s="60"/>
+      <c r="W19" s="60"/>
       <c r="X19" s="12"/>
       <c r="Y19" s="12"/>
       <c r="Z19" s="12"/>
@@ -3338,498 +3338,517 @@
       <c r="AB19" s="13"/>
     </row>
     <row r="20" spans="1:28" ht="16" x14ac:dyDescent="0.15">
-      <c r="A20" s="61" t="s">
+      <c r="A20" s="25" t="s">
         <v>41</v>
       </c>
-      <c r="B20" s="62"/>
-      <c r="C20" s="62"/>
-      <c r="D20" s="62"/>
-      <c r="E20" s="62"/>
-      <c r="F20" s="62"/>
-      <c r="G20" s="62"/>
-      <c r="H20" s="62"/>
-      <c r="I20" s="62"/>
-      <c r="J20" s="62"/>
-      <c r="K20" s="62"/>
-      <c r="L20" s="62"/>
-      <c r="M20" s="62"/>
-      <c r="N20" s="62"/>
-      <c r="O20" s="62"/>
-      <c r="P20" s="62"/>
-      <c r="Q20" s="62"/>
-      <c r="R20" s="62"/>
-      <c r="S20" s="62"/>
-      <c r="T20" s="62"/>
-      <c r="U20" s="62"/>
-      <c r="V20" s="62"/>
-      <c r="W20" s="62"/>
-      <c r="X20" s="62"/>
-      <c r="Y20" s="62"/>
-      <c r="Z20" s="62"/>
-      <c r="AA20" s="62"/>
-      <c r="AB20" s="63"/>
+      <c r="B20" s="26"/>
+      <c r="C20" s="26"/>
+      <c r="D20" s="26"/>
+      <c r="E20" s="26"/>
+      <c r="F20" s="26"/>
+      <c r="G20" s="26"/>
+      <c r="H20" s="26"/>
+      <c r="I20" s="26"/>
+      <c r="J20" s="26"/>
+      <c r="K20" s="26"/>
+      <c r="L20" s="26"/>
+      <c r="M20" s="26"/>
+      <c r="N20" s="26"/>
+      <c r="O20" s="26"/>
+      <c r="P20" s="26"/>
+      <c r="Q20" s="26"/>
+      <c r="R20" s="26"/>
+      <c r="S20" s="26"/>
+      <c r="T20" s="26"/>
+      <c r="U20" s="26"/>
+      <c r="V20" s="26"/>
+      <c r="W20" s="26"/>
+      <c r="X20" s="26"/>
+      <c r="Y20" s="26"/>
+      <c r="Z20" s="26"/>
+      <c r="AA20" s="26"/>
+      <c r="AB20" s="27"/>
     </row>
     <row r="21" spans="1:28" x14ac:dyDescent="0.15">
-      <c r="A21" s="61"/>
-      <c r="B21" s="62"/>
-      <c r="C21" s="62"/>
-      <c r="D21" s="62"/>
-      <c r="E21" s="62"/>
-      <c r="F21" s="62"/>
-      <c r="G21" s="62"/>
-      <c r="H21" s="62"/>
-      <c r="I21" s="62"/>
-      <c r="J21" s="62"/>
-      <c r="K21" s="62"/>
-      <c r="L21" s="62"/>
-      <c r="M21" s="62"/>
-      <c r="N21" s="62"/>
-      <c r="O21" s="62"/>
-      <c r="P21" s="62"/>
-      <c r="Q21" s="62"/>
-      <c r="R21" s="62"/>
-      <c r="S21" s="62"/>
-      <c r="T21" s="62"/>
-      <c r="U21" s="62"/>
-      <c r="V21" s="62"/>
-      <c r="W21" s="62"/>
-      <c r="X21" s="62"/>
-      <c r="Y21" s="62"/>
-      <c r="Z21" s="62"/>
-      <c r="AA21" s="62"/>
-      <c r="AB21" s="63"/>
+      <c r="A21" s="25"/>
+      <c r="B21" s="26"/>
+      <c r="C21" s="26"/>
+      <c r="D21" s="26"/>
+      <c r="E21" s="26"/>
+      <c r="F21" s="26"/>
+      <c r="G21" s="26"/>
+      <c r="H21" s="26"/>
+      <c r="I21" s="26"/>
+      <c r="J21" s="26"/>
+      <c r="K21" s="26"/>
+      <c r="L21" s="26"/>
+      <c r="M21" s="26"/>
+      <c r="N21" s="26"/>
+      <c r="O21" s="26"/>
+      <c r="P21" s="26"/>
+      <c r="Q21" s="26"/>
+      <c r="R21" s="26"/>
+      <c r="S21" s="26"/>
+      <c r="T21" s="26"/>
+      <c r="U21" s="26"/>
+      <c r="V21" s="26"/>
+      <c r="W21" s="26"/>
+      <c r="X21" s="26"/>
+      <c r="Y21" s="26"/>
+      <c r="Z21" s="26"/>
+      <c r="AA21" s="26"/>
+      <c r="AB21" s="27"/>
     </row>
     <row r="22" spans="1:28" x14ac:dyDescent="0.15">
-      <c r="A22" s="61"/>
-      <c r="B22" s="62"/>
-      <c r="C22" s="62"/>
-      <c r="D22" s="62"/>
-      <c r="E22" s="62"/>
-      <c r="F22" s="62"/>
-      <c r="G22" s="62"/>
-      <c r="H22" s="62"/>
-      <c r="I22" s="62"/>
-      <c r="J22" s="62"/>
-      <c r="K22" s="62"/>
-      <c r="L22" s="62"/>
-      <c r="M22" s="62"/>
-      <c r="N22" s="62"/>
-      <c r="O22" s="62"/>
-      <c r="P22" s="62"/>
-      <c r="Q22" s="62"/>
-      <c r="R22" s="62"/>
-      <c r="S22" s="62"/>
-      <c r="T22" s="62"/>
-      <c r="U22" s="62"/>
-      <c r="V22" s="62"/>
-      <c r="W22" s="62"/>
-      <c r="X22" s="62"/>
-      <c r="Y22" s="62"/>
-      <c r="Z22" s="62"/>
-      <c r="AA22" s="62"/>
-      <c r="AB22" s="63"/>
+      <c r="A22" s="25"/>
+      <c r="B22" s="26"/>
+      <c r="C22" s="26"/>
+      <c r="D22" s="26"/>
+      <c r="E22" s="26"/>
+      <c r="F22" s="26"/>
+      <c r="G22" s="26"/>
+      <c r="H22" s="26"/>
+      <c r="I22" s="26"/>
+      <c r="J22" s="26"/>
+      <c r="K22" s="26"/>
+      <c r="L22" s="26"/>
+      <c r="M22" s="26"/>
+      <c r="N22" s="26"/>
+      <c r="O22" s="26"/>
+      <c r="P22" s="26"/>
+      <c r="Q22" s="26"/>
+      <c r="R22" s="26"/>
+      <c r="S22" s="26"/>
+      <c r="T22" s="26"/>
+      <c r="U22" s="26"/>
+      <c r="V22" s="26"/>
+      <c r="W22" s="26"/>
+      <c r="X22" s="26"/>
+      <c r="Y22" s="26"/>
+      <c r="Z22" s="26"/>
+      <c r="AA22" s="26"/>
+      <c r="AB22" s="27"/>
     </row>
     <row r="23" spans="1:28" x14ac:dyDescent="0.15">
-      <c r="A23" s="61"/>
-      <c r="B23" s="62"/>
-      <c r="C23" s="62"/>
-      <c r="D23" s="62"/>
-      <c r="E23" s="62"/>
-      <c r="F23" s="62"/>
-      <c r="G23" s="62"/>
-      <c r="H23" s="62"/>
-      <c r="I23" s="62"/>
-      <c r="J23" s="62"/>
-      <c r="K23" s="62"/>
-      <c r="L23" s="62"/>
-      <c r="M23" s="62"/>
-      <c r="N23" s="62"/>
-      <c r="O23" s="62"/>
-      <c r="P23" s="62"/>
-      <c r="Q23" s="62"/>
-      <c r="R23" s="62"/>
-      <c r="S23" s="62"/>
-      <c r="T23" s="62"/>
-      <c r="U23" s="62"/>
-      <c r="V23" s="62"/>
-      <c r="W23" s="62"/>
-      <c r="X23" s="62"/>
-      <c r="Y23" s="62"/>
-      <c r="Z23" s="62"/>
-      <c r="AA23" s="62"/>
-      <c r="AB23" s="63"/>
+      <c r="A23" s="25"/>
+      <c r="B23" s="26"/>
+      <c r="C23" s="26"/>
+      <c r="D23" s="26"/>
+      <c r="E23" s="26"/>
+      <c r="F23" s="26"/>
+      <c r="G23" s="26"/>
+      <c r="H23" s="26"/>
+      <c r="I23" s="26"/>
+      <c r="J23" s="26"/>
+      <c r="K23" s="26"/>
+      <c r="L23" s="26"/>
+      <c r="M23" s="26"/>
+      <c r="N23" s="26"/>
+      <c r="O23" s="26"/>
+      <c r="P23" s="26"/>
+      <c r="Q23" s="26"/>
+      <c r="R23" s="26"/>
+      <c r="S23" s="26"/>
+      <c r="T23" s="26"/>
+      <c r="U23" s="26"/>
+      <c r="V23" s="26"/>
+      <c r="W23" s="26"/>
+      <c r="X23" s="26"/>
+      <c r="Y23" s="26"/>
+      <c r="Z23" s="26"/>
+      <c r="AA23" s="26"/>
+      <c r="AB23" s="27"/>
     </row>
     <row r="24" spans="1:28" x14ac:dyDescent="0.15">
-      <c r="A24" s="61"/>
-      <c r="B24" s="62"/>
-      <c r="C24" s="62"/>
-      <c r="D24" s="62"/>
-      <c r="E24" s="62"/>
-      <c r="F24" s="62"/>
-      <c r="G24" s="62"/>
-      <c r="H24" s="62"/>
-      <c r="I24" s="62"/>
-      <c r="J24" s="62"/>
-      <c r="K24" s="62"/>
-      <c r="L24" s="62"/>
-      <c r="M24" s="62"/>
-      <c r="N24" s="62"/>
-      <c r="O24" s="62"/>
-      <c r="P24" s="62"/>
-      <c r="Q24" s="62"/>
-      <c r="R24" s="62"/>
-      <c r="S24" s="62"/>
-      <c r="T24" s="62"/>
-      <c r="U24" s="62"/>
-      <c r="V24" s="62"/>
-      <c r="W24" s="62"/>
-      <c r="X24" s="62"/>
-      <c r="Y24" s="62"/>
-      <c r="Z24" s="62"/>
-      <c r="AA24" s="62"/>
-      <c r="AB24" s="63"/>
+      <c r="A24" s="25"/>
+      <c r="B24" s="26"/>
+      <c r="C24" s="26"/>
+      <c r="D24" s="26"/>
+      <c r="E24" s="26"/>
+      <c r="F24" s="26"/>
+      <c r="G24" s="26"/>
+      <c r="H24" s="26"/>
+      <c r="I24" s="26"/>
+      <c r="J24" s="26"/>
+      <c r="K24" s="26"/>
+      <c r="L24" s="26"/>
+      <c r="M24" s="26"/>
+      <c r="N24" s="26"/>
+      <c r="O24" s="26"/>
+      <c r="P24" s="26"/>
+      <c r="Q24" s="26"/>
+      <c r="R24" s="26"/>
+      <c r="S24" s="26"/>
+      <c r="T24" s="26"/>
+      <c r="U24" s="26"/>
+      <c r="V24" s="26"/>
+      <c r="W24" s="26"/>
+      <c r="X24" s="26"/>
+      <c r="Y24" s="26"/>
+      <c r="Z24" s="26"/>
+      <c r="AA24" s="26"/>
+      <c r="AB24" s="27"/>
     </row>
     <row r="25" spans="1:28" x14ac:dyDescent="0.15">
-      <c r="A25" s="61"/>
-      <c r="B25" s="62"/>
-      <c r="C25" s="62"/>
-      <c r="D25" s="62"/>
-      <c r="E25" s="62"/>
-      <c r="F25" s="62"/>
-      <c r="G25" s="62"/>
-      <c r="H25" s="62"/>
-      <c r="I25" s="62"/>
-      <c r="J25" s="62"/>
-      <c r="K25" s="62"/>
-      <c r="L25" s="62"/>
-      <c r="M25" s="62"/>
-      <c r="N25" s="62"/>
-      <c r="O25" s="62"/>
-      <c r="P25" s="62"/>
-      <c r="Q25" s="62"/>
-      <c r="R25" s="62"/>
-      <c r="S25" s="62"/>
-      <c r="T25" s="62"/>
-      <c r="U25" s="62"/>
-      <c r="V25" s="62"/>
-      <c r="W25" s="62"/>
-      <c r="X25" s="62"/>
-      <c r="Y25" s="62"/>
-      <c r="Z25" s="62"/>
-      <c r="AA25" s="62"/>
-      <c r="AB25" s="63"/>
+      <c r="A25" s="25"/>
+      <c r="B25" s="26"/>
+      <c r="C25" s="26"/>
+      <c r="D25" s="26"/>
+      <c r="E25" s="26"/>
+      <c r="F25" s="26"/>
+      <c r="G25" s="26"/>
+      <c r="H25" s="26"/>
+      <c r="I25" s="26"/>
+      <c r="J25" s="26"/>
+      <c r="K25" s="26"/>
+      <c r="L25" s="26"/>
+      <c r="M25" s="26"/>
+      <c r="N25" s="26"/>
+      <c r="O25" s="26"/>
+      <c r="P25" s="26"/>
+      <c r="Q25" s="26"/>
+      <c r="R25" s="26"/>
+      <c r="S25" s="26"/>
+      <c r="T25" s="26"/>
+      <c r="U25" s="26"/>
+      <c r="V25" s="26"/>
+      <c r="W25" s="26"/>
+      <c r="X25" s="26"/>
+      <c r="Y25" s="26"/>
+      <c r="Z25" s="26"/>
+      <c r="AA25" s="26"/>
+      <c r="AB25" s="27"/>
     </row>
     <row r="26" spans="1:28" x14ac:dyDescent="0.15">
-      <c r="A26" s="61"/>
-      <c r="B26" s="62"/>
-      <c r="C26" s="62"/>
-      <c r="D26" s="62"/>
-      <c r="E26" s="62"/>
-      <c r="F26" s="62"/>
-      <c r="G26" s="62"/>
-      <c r="H26" s="62"/>
-      <c r="I26" s="62"/>
-      <c r="J26" s="62"/>
-      <c r="K26" s="62"/>
-      <c r="L26" s="62"/>
-      <c r="M26" s="62"/>
-      <c r="N26" s="62"/>
-      <c r="O26" s="62"/>
-      <c r="P26" s="62"/>
-      <c r="Q26" s="62"/>
-      <c r="R26" s="62"/>
-      <c r="S26" s="62"/>
-      <c r="T26" s="62"/>
-      <c r="U26" s="62"/>
-      <c r="V26" s="62"/>
-      <c r="W26" s="62"/>
-      <c r="X26" s="62"/>
-      <c r="Y26" s="62"/>
-      <c r="Z26" s="62"/>
-      <c r="AA26" s="62"/>
-      <c r="AB26" s="63"/>
+      <c r="A26" s="25"/>
+      <c r="B26" s="26"/>
+      <c r="C26" s="26"/>
+      <c r="D26" s="26"/>
+      <c r="E26" s="26"/>
+      <c r="F26" s="26"/>
+      <c r="G26" s="26"/>
+      <c r="H26" s="26"/>
+      <c r="I26" s="26"/>
+      <c r="J26" s="26"/>
+      <c r="K26" s="26"/>
+      <c r="L26" s="26"/>
+      <c r="M26" s="26"/>
+      <c r="N26" s="26"/>
+      <c r="O26" s="26"/>
+      <c r="P26" s="26"/>
+      <c r="Q26" s="26"/>
+      <c r="R26" s="26"/>
+      <c r="S26" s="26"/>
+      <c r="T26" s="26"/>
+      <c r="U26" s="26"/>
+      <c r="V26" s="26"/>
+      <c r="W26" s="26"/>
+      <c r="X26" s="26"/>
+      <c r="Y26" s="26"/>
+      <c r="Z26" s="26"/>
+      <c r="AA26" s="26"/>
+      <c r="AB26" s="27"/>
     </row>
     <row r="27" spans="1:28" x14ac:dyDescent="0.15">
-      <c r="A27" s="61"/>
-      <c r="B27" s="62"/>
-      <c r="C27" s="62"/>
-      <c r="D27" s="62"/>
-      <c r="E27" s="62"/>
-      <c r="F27" s="62"/>
-      <c r="G27" s="62"/>
-      <c r="H27" s="62"/>
-      <c r="I27" s="62"/>
-      <c r="J27" s="62"/>
-      <c r="K27" s="62"/>
-      <c r="L27" s="62"/>
-      <c r="M27" s="62"/>
-      <c r="N27" s="62"/>
-      <c r="O27" s="62"/>
-      <c r="P27" s="62"/>
-      <c r="Q27" s="62"/>
-      <c r="R27" s="62"/>
-      <c r="S27" s="62"/>
-      <c r="T27" s="62"/>
-      <c r="U27" s="62"/>
-      <c r="V27" s="62"/>
-      <c r="W27" s="62"/>
-      <c r="X27" s="62"/>
-      <c r="Y27" s="62"/>
-      <c r="Z27" s="62"/>
-      <c r="AA27" s="62"/>
-      <c r="AB27" s="63"/>
+      <c r="A27" s="25"/>
+      <c r="B27" s="26"/>
+      <c r="C27" s="26"/>
+      <c r="D27" s="26"/>
+      <c r="E27" s="26"/>
+      <c r="F27" s="26"/>
+      <c r="G27" s="26"/>
+      <c r="H27" s="26"/>
+      <c r="I27" s="26"/>
+      <c r="J27" s="26"/>
+      <c r="K27" s="26"/>
+      <c r="L27" s="26"/>
+      <c r="M27" s="26"/>
+      <c r="N27" s="26"/>
+      <c r="O27" s="26"/>
+      <c r="P27" s="26"/>
+      <c r="Q27" s="26"/>
+      <c r="R27" s="26"/>
+      <c r="S27" s="26"/>
+      <c r="T27" s="26"/>
+      <c r="U27" s="26"/>
+      <c r="V27" s="26"/>
+      <c r="W27" s="26"/>
+      <c r="X27" s="26"/>
+      <c r="Y27" s="26"/>
+      <c r="Z27" s="26"/>
+      <c r="AA27" s="26"/>
+      <c r="AB27" s="27"/>
     </row>
     <row r="28" spans="1:28" x14ac:dyDescent="0.15">
-      <c r="A28" s="61"/>
-      <c r="B28" s="62"/>
-      <c r="C28" s="62"/>
-      <c r="D28" s="62"/>
-      <c r="E28" s="62"/>
-      <c r="F28" s="62"/>
-      <c r="G28" s="62"/>
-      <c r="H28" s="62"/>
-      <c r="I28" s="62"/>
-      <c r="J28" s="62"/>
-      <c r="K28" s="62"/>
-      <c r="L28" s="62"/>
-      <c r="M28" s="62"/>
-      <c r="N28" s="62"/>
-      <c r="O28" s="62"/>
-      <c r="P28" s="62"/>
-      <c r="Q28" s="62"/>
-      <c r="R28" s="62"/>
-      <c r="S28" s="62"/>
-      <c r="T28" s="62"/>
-      <c r="U28" s="62"/>
-      <c r="V28" s="62"/>
-      <c r="W28" s="62"/>
-      <c r="X28" s="62"/>
-      <c r="Y28" s="62"/>
-      <c r="Z28" s="62"/>
-      <c r="AA28" s="62"/>
-      <c r="AB28" s="63"/>
+      <c r="A28" s="25"/>
+      <c r="B28" s="26"/>
+      <c r="C28" s="26"/>
+      <c r="D28" s="26"/>
+      <c r="E28" s="26"/>
+      <c r="F28" s="26"/>
+      <c r="G28" s="26"/>
+      <c r="H28" s="26"/>
+      <c r="I28" s="26"/>
+      <c r="J28" s="26"/>
+      <c r="K28" s="26"/>
+      <c r="L28" s="26"/>
+      <c r="M28" s="26"/>
+      <c r="N28" s="26"/>
+      <c r="O28" s="26"/>
+      <c r="P28" s="26"/>
+      <c r="Q28" s="26"/>
+      <c r="R28" s="26"/>
+      <c r="S28" s="26"/>
+      <c r="T28" s="26"/>
+      <c r="U28" s="26"/>
+      <c r="V28" s="26"/>
+      <c r="W28" s="26"/>
+      <c r="X28" s="26"/>
+      <c r="Y28" s="26"/>
+      <c r="Z28" s="26"/>
+      <c r="AA28" s="26"/>
+      <c r="AB28" s="27"/>
     </row>
     <row r="29" spans="1:28" x14ac:dyDescent="0.15">
-      <c r="A29" s="85"/>
-      <c r="B29" s="86"/>
-      <c r="C29" s="86"/>
-      <c r="D29" s="86"/>
-      <c r="E29" s="86"/>
-      <c r="F29" s="86"/>
-      <c r="G29" s="86"/>
-      <c r="H29" s="86"/>
-      <c r="I29" s="86"/>
-      <c r="J29" s="86"/>
-      <c r="K29" s="86"/>
-      <c r="L29" s="86"/>
-      <c r="M29" s="86"/>
-      <c r="N29" s="86"/>
-      <c r="O29" s="86"/>
-      <c r="P29" s="86"/>
-      <c r="Q29" s="86"/>
-      <c r="R29" s="86"/>
-      <c r="S29" s="86"/>
-      <c r="T29" s="86"/>
-      <c r="U29" s="86"/>
-      <c r="V29" s="86"/>
-      <c r="W29" s="86"/>
-      <c r="X29" s="86"/>
-      <c r="Y29" s="86"/>
-      <c r="Z29" s="86"/>
-      <c r="AA29" s="86"/>
-      <c r="AB29" s="87"/>
+      <c r="A29" s="28"/>
+      <c r="B29" s="29"/>
+      <c r="C29" s="29"/>
+      <c r="D29" s="29"/>
+      <c r="E29" s="29"/>
+      <c r="F29" s="29"/>
+      <c r="G29" s="29"/>
+      <c r="H29" s="29"/>
+      <c r="I29" s="29"/>
+      <c r="J29" s="29"/>
+      <c r="K29" s="29"/>
+      <c r="L29" s="29"/>
+      <c r="M29" s="29"/>
+      <c r="N29" s="29"/>
+      <c r="O29" s="29"/>
+      <c r="P29" s="29"/>
+      <c r="Q29" s="29"/>
+      <c r="R29" s="29"/>
+      <c r="S29" s="29"/>
+      <c r="T29" s="29"/>
+      <c r="U29" s="29"/>
+      <c r="V29" s="29"/>
+      <c r="W29" s="29"/>
+      <c r="X29" s="29"/>
+      <c r="Y29" s="29"/>
+      <c r="Z29" s="29"/>
+      <c r="AA29" s="29"/>
+      <c r="AB29" s="30"/>
     </row>
     <row r="30" spans="1:28" x14ac:dyDescent="0.15">
-      <c r="A30" s="88" t="s">
+      <c r="A30" s="31" t="s">
         <v>42</v>
       </c>
-      <c r="B30" s="89"/>
-      <c r="C30" s="89"/>
-      <c r="D30" s="89"/>
-      <c r="E30" s="89"/>
-      <c r="F30" s="89"/>
-      <c r="G30" s="89"/>
-      <c r="H30" s="89"/>
-      <c r="I30" s="89"/>
-      <c r="J30" s="89"/>
-      <c r="K30" s="89"/>
-      <c r="L30" s="89"/>
-      <c r="M30" s="89"/>
-      <c r="N30" s="89"/>
-      <c r="O30" s="89"/>
-      <c r="P30" s="89"/>
-      <c r="Q30" s="89"/>
-      <c r="R30" s="89"/>
-      <c r="S30" s="89"/>
-      <c r="T30" s="89"/>
+      <c r="B30" s="32"/>
+      <c r="C30" s="32"/>
+      <c r="D30" s="32"/>
+      <c r="E30" s="32"/>
+      <c r="F30" s="32"/>
+      <c r="G30" s="32"/>
+      <c r="H30" s="32"/>
+      <c r="I30" s="32"/>
+      <c r="J30" s="32"/>
+      <c r="K30" s="32"/>
+      <c r="L30" s="32"/>
+      <c r="M30" s="32"/>
+      <c r="N30" s="32"/>
+      <c r="O30" s="32"/>
+      <c r="P30" s="32"/>
+      <c r="Q30" s="32"/>
+      <c r="R30" s="32"/>
+      <c r="S30" s="32"/>
+      <c r="T30" s="32"/>
       <c r="U30" s="14" t="s">
-        <v>58</v>
-      </c>
-      <c r="V30" s="90" t="s">
+        <v>57</v>
+      </c>
+      <c r="V30" s="33" t="s">
         <v>43</v>
       </c>
-      <c r="W30" s="90"/>
-      <c r="X30" s="90"/>
-      <c r="Y30" s="90"/>
-      <c r="Z30" s="90"/>
-      <c r="AA30" s="90"/>
-      <c r="AB30" s="91"/>
+      <c r="W30" s="33"/>
+      <c r="X30" s="33"/>
+      <c r="Y30" s="33"/>
+      <c r="Z30" s="33"/>
+      <c r="AA30" s="33"/>
+      <c r="AB30" s="34"/>
     </row>
     <row r="31" spans="1:28" x14ac:dyDescent="0.15">
-      <c r="A31" s="92" t="s">
+      <c r="A31" s="35" t="s">
         <v>44</v>
       </c>
-      <c r="B31" s="93"/>
-      <c r="C31" s="93"/>
-      <c r="D31" s="93"/>
-      <c r="E31" s="93"/>
-      <c r="F31" s="93"/>
-      <c r="G31" s="93"/>
-      <c r="H31" s="93"/>
-      <c r="I31" s="93"/>
-      <c r="J31" s="93"/>
-      <c r="K31" s="93"/>
-      <c r="L31" s="93"/>
-      <c r="M31" s="93"/>
-      <c r="N31" s="93"/>
-      <c r="O31" s="93"/>
-      <c r="P31" s="93"/>
-      <c r="Q31" s="93"/>
-      <c r="R31" s="93"/>
-      <c r="S31" s="93"/>
-      <c r="T31" s="93"/>
-      <c r="U31" s="93"/>
-      <c r="V31" s="93"/>
-      <c r="W31" s="93"/>
-      <c r="X31" s="93"/>
-      <c r="Y31" s="93"/>
-      <c r="Z31" s="93"/>
-      <c r="AA31" s="93"/>
-      <c r="AB31" s="94"/>
+      <c r="B31" s="36"/>
+      <c r="C31" s="36"/>
+      <c r="D31" s="36"/>
+      <c r="E31" s="36"/>
+      <c r="F31" s="36"/>
+      <c r="G31" s="36"/>
+      <c r="H31" s="36"/>
+      <c r="I31" s="36"/>
+      <c r="J31" s="36"/>
+      <c r="K31" s="36"/>
+      <c r="L31" s="36"/>
+      <c r="M31" s="36"/>
+      <c r="N31" s="36"/>
+      <c r="O31" s="36"/>
+      <c r="P31" s="36"/>
+      <c r="Q31" s="36"/>
+      <c r="R31" s="36"/>
+      <c r="S31" s="36"/>
+      <c r="T31" s="36"/>
+      <c r="U31" s="36"/>
+      <c r="V31" s="36"/>
+      <c r="W31" s="36"/>
+      <c r="X31" s="36"/>
+      <c r="Y31" s="36"/>
+      <c r="Z31" s="36"/>
+      <c r="AA31" s="36"/>
+      <c r="AB31" s="37"/>
     </row>
     <row r="32" spans="1:28" x14ac:dyDescent="0.15">
-      <c r="A32" s="95" t="s">
+      <c r="A32" s="38" t="s">
         <v>45</v>
       </c>
-      <c r="B32" s="54"/>
-      <c r="C32" s="54"/>
-      <c r="D32" s="54"/>
-      <c r="E32" s="54"/>
-      <c r="F32" s="54"/>
-      <c r="G32" s="54"/>
-      <c r="H32" s="54"/>
-      <c r="I32" s="54"/>
-      <c r="J32" s="53" t="s">
-        <v>59</v>
-      </c>
-      <c r="K32" s="54"/>
-      <c r="L32" s="54"/>
-      <c r="M32" s="54"/>
-      <c r="N32" s="54"/>
-      <c r="O32" s="54"/>
-      <c r="P32" s="54"/>
-      <c r="Q32" s="54"/>
-      <c r="R32" s="54"/>
-      <c r="S32" s="54"/>
-      <c r="T32" s="54"/>
-      <c r="U32" s="54"/>
-      <c r="V32" s="54"/>
-      <c r="W32" s="54"/>
-      <c r="X32" s="54"/>
-      <c r="Y32" s="54"/>
-      <c r="Z32" s="54"/>
-      <c r="AA32" s="54"/>
-      <c r="AB32" s="96"/>
+      <c r="B32" s="20"/>
+      <c r="C32" s="20"/>
+      <c r="D32" s="20"/>
+      <c r="E32" s="20"/>
+      <c r="F32" s="20"/>
+      <c r="G32" s="20"/>
+      <c r="H32" s="20"/>
+      <c r="I32" s="20"/>
+      <c r="J32" s="19" t="s">
+        <v>58</v>
+      </c>
+      <c r="K32" s="20"/>
+      <c r="L32" s="20"/>
+      <c r="M32" s="20"/>
+      <c r="N32" s="20"/>
+      <c r="O32" s="20"/>
+      <c r="P32" s="20"/>
+      <c r="Q32" s="20"/>
+      <c r="R32" s="20"/>
+      <c r="S32" s="20"/>
+      <c r="T32" s="20"/>
+      <c r="U32" s="20"/>
+      <c r="V32" s="20"/>
+      <c r="W32" s="20"/>
+      <c r="X32" s="20"/>
+      <c r="Y32" s="20"/>
+      <c r="Z32" s="20"/>
+      <c r="AA32" s="20"/>
+      <c r="AB32" s="22"/>
     </row>
     <row r="33" spans="1:28" x14ac:dyDescent="0.15">
-      <c r="A33" s="97" t="s">
+      <c r="A33" s="15" t="s">
         <v>46</v>
       </c>
-      <c r="B33" s="98"/>
-      <c r="C33" s="98"/>
-      <c r="D33" s="98"/>
-      <c r="E33" s="98"/>
-      <c r="F33" s="98"/>
-      <c r="G33" s="98"/>
-      <c r="H33" s="98"/>
-      <c r="I33" s="98"/>
-      <c r="J33" s="53" t="s">
+      <c r="B33" s="16"/>
+      <c r="C33" s="16"/>
+      <c r="D33" s="16"/>
+      <c r="E33" s="16"/>
+      <c r="F33" s="16"/>
+      <c r="G33" s="16"/>
+      <c r="H33" s="16"/>
+      <c r="I33" s="16"/>
+      <c r="J33" s="19" t="s">
         <v>47</v>
       </c>
-      <c r="K33" s="54"/>
-      <c r="L33" s="54"/>
-      <c r="M33" s="54"/>
-      <c r="N33" s="54"/>
-      <c r="O33" s="54"/>
-      <c r="P33" s="54"/>
-      <c r="Q33" s="54"/>
-      <c r="R33" s="54"/>
-      <c r="S33" s="54"/>
-      <c r="T33" s="54"/>
-      <c r="U33" s="101"/>
-      <c r="V33" s="53" t="s">
+      <c r="K33" s="20"/>
+      <c r="L33" s="20"/>
+      <c r="M33" s="20"/>
+      <c r="N33" s="20"/>
+      <c r="O33" s="20"/>
+      <c r="P33" s="20"/>
+      <c r="Q33" s="20"/>
+      <c r="R33" s="20"/>
+      <c r="S33" s="20"/>
+      <c r="T33" s="20"/>
+      <c r="U33" s="21"/>
+      <c r="V33" s="19" t="s">
         <v>48</v>
       </c>
-      <c r="W33" s="54"/>
-      <c r="X33" s="101"/>
-      <c r="Y33" s="53" t="s">
+      <c r="W33" s="20"/>
+      <c r="X33" s="21"/>
+      <c r="Y33" s="19" t="s">
         <v>49</v>
       </c>
-      <c r="Z33" s="54"/>
-      <c r="AA33" s="54"/>
-      <c r="AB33" s="96"/>
+      <c r="Z33" s="20"/>
+      <c r="AA33" s="20"/>
+      <c r="AB33" s="22"/>
     </row>
     <row r="34" spans="1:28" ht="16" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A34" s="99"/>
-      <c r="B34" s="100"/>
-      <c r="C34" s="100"/>
-      <c r="D34" s="100"/>
-      <c r="E34" s="100"/>
-      <c r="F34" s="100"/>
-      <c r="G34" s="100"/>
-      <c r="H34" s="100"/>
-      <c r="I34" s="100"/>
-      <c r="J34" s="102" t="s">
+      <c r="A34" s="17"/>
+      <c r="B34" s="18"/>
+      <c r="C34" s="18"/>
+      <c r="D34" s="18"/>
+      <c r="E34" s="18"/>
+      <c r="F34" s="18"/>
+      <c r="G34" s="18"/>
+      <c r="H34" s="18"/>
+      <c r="I34" s="18"/>
+      <c r="J34" s="23" t="s">
         <v>50</v>
       </c>
-      <c r="K34" s="102"/>
-      <c r="L34" s="102"/>
-      <c r="M34" s="102"/>
-      <c r="N34" s="102"/>
-      <c r="O34" s="102"/>
-      <c r="P34" s="102"/>
-      <c r="Q34" s="102"/>
-      <c r="R34" s="102"/>
-      <c r="S34" s="102"/>
-      <c r="T34" s="102"/>
-      <c r="U34" s="102"/>
-      <c r="V34" s="102" t="s">
+      <c r="K34" s="23"/>
+      <c r="L34" s="23"/>
+      <c r="M34" s="23"/>
+      <c r="N34" s="23"/>
+      <c r="O34" s="23"/>
+      <c r="P34" s="23"/>
+      <c r="Q34" s="23"/>
+      <c r="R34" s="23"/>
+      <c r="S34" s="23"/>
+      <c r="T34" s="23"/>
+      <c r="U34" s="23"/>
+      <c r="V34" s="23" t="s">
         <v>51</v>
       </c>
-      <c r="W34" s="102"/>
-      <c r="X34" s="102"/>
-      <c r="Y34" s="102" t="s">
+      <c r="W34" s="23"/>
+      <c r="X34" s="23"/>
+      <c r="Y34" s="23" t="s">
         <v>52</v>
       </c>
-      <c r="Z34" s="102"/>
-      <c r="AA34" s="102"/>
-      <c r="AB34" s="103"/>
+      <c r="Z34" s="23"/>
+      <c r="AA34" s="23"/>
+      <c r="AB34" s="24"/>
     </row>
   </sheetData>
   <mergeCells count="59">
-    <mergeCell ref="A33:I34"/>
-    <mergeCell ref="J33:U33"/>
-    <mergeCell ref="V33:X33"/>
-    <mergeCell ref="Y33:AB33"/>
-    <mergeCell ref="J34:U34"/>
-    <mergeCell ref="V34:X34"/>
-    <mergeCell ref="Y34:AB34"/>
-    <mergeCell ref="A21:AB29"/>
-    <mergeCell ref="A30:T30"/>
-    <mergeCell ref="V30:AB30"/>
-    <mergeCell ref="A31:AB31"/>
-    <mergeCell ref="A32:I32"/>
-    <mergeCell ref="J32:AB32"/>
+    <mergeCell ref="A6:V6"/>
+    <mergeCell ref="W6:AB6"/>
+    <mergeCell ref="A1:AB2"/>
+    <mergeCell ref="A3:AB3"/>
+    <mergeCell ref="A4:O4"/>
+    <mergeCell ref="P4:AB4"/>
+    <mergeCell ref="A5:AB5"/>
+    <mergeCell ref="A7:Z7"/>
+    <mergeCell ref="A8:A9"/>
+    <mergeCell ref="B8:T8"/>
+    <mergeCell ref="U8:W9"/>
+    <mergeCell ref="X8:AB9"/>
+    <mergeCell ref="C9:D9"/>
+    <mergeCell ref="F9:H9"/>
+    <mergeCell ref="J9:M9"/>
+    <mergeCell ref="Q9:S9"/>
+    <mergeCell ref="B10:T10"/>
+    <mergeCell ref="V10:W10"/>
+    <mergeCell ref="Y10:AB10"/>
+    <mergeCell ref="B11:K11"/>
+    <mergeCell ref="L11:T11"/>
+    <mergeCell ref="V11:W11"/>
+    <mergeCell ref="Y11:AB11"/>
+    <mergeCell ref="A12:A13"/>
+    <mergeCell ref="B12:K12"/>
+    <mergeCell ref="L12:T12"/>
+    <mergeCell ref="V12:W12"/>
+    <mergeCell ref="Y12:AB12"/>
+    <mergeCell ref="B13:K13"/>
+    <mergeCell ref="L13:T13"/>
+    <mergeCell ref="V13:W13"/>
+    <mergeCell ref="Y13:AB13"/>
     <mergeCell ref="A20:AB20"/>
     <mergeCell ref="A14:M14"/>
     <mergeCell ref="N14:AB14"/>
@@ -3844,38 +3863,19 @@
     <mergeCell ref="U17:X17"/>
     <mergeCell ref="A18:AB18"/>
     <mergeCell ref="A19:W19"/>
-    <mergeCell ref="A12:A13"/>
-    <mergeCell ref="B12:K12"/>
-    <mergeCell ref="L12:T12"/>
-    <mergeCell ref="V12:W12"/>
-    <mergeCell ref="Y12:AB12"/>
-    <mergeCell ref="B13:K13"/>
-    <mergeCell ref="L13:T13"/>
-    <mergeCell ref="V13:W13"/>
-    <mergeCell ref="Y13:AB13"/>
-    <mergeCell ref="B10:T10"/>
-    <mergeCell ref="V10:W10"/>
-    <mergeCell ref="Y10:AB10"/>
-    <mergeCell ref="B11:K11"/>
-    <mergeCell ref="L11:T11"/>
-    <mergeCell ref="V11:W11"/>
-    <mergeCell ref="Y11:AB11"/>
-    <mergeCell ref="A7:Z7"/>
-    <mergeCell ref="A8:A9"/>
-    <mergeCell ref="B8:T8"/>
-    <mergeCell ref="U8:W9"/>
-    <mergeCell ref="X8:AB9"/>
-    <mergeCell ref="C9:D9"/>
-    <mergeCell ref="F9:H9"/>
-    <mergeCell ref="J9:M9"/>
-    <mergeCell ref="Q9:S9"/>
-    <mergeCell ref="A6:V6"/>
-    <mergeCell ref="W6:AB6"/>
-    <mergeCell ref="A1:AB2"/>
-    <mergeCell ref="A3:AB3"/>
-    <mergeCell ref="A4:O4"/>
-    <mergeCell ref="P4:AB4"/>
-    <mergeCell ref="A5:AB5"/>
+    <mergeCell ref="A21:AB29"/>
+    <mergeCell ref="A30:T30"/>
+    <mergeCell ref="V30:AB30"/>
+    <mergeCell ref="A31:AB31"/>
+    <mergeCell ref="A32:I32"/>
+    <mergeCell ref="J32:AB32"/>
+    <mergeCell ref="A33:I34"/>
+    <mergeCell ref="J33:U33"/>
+    <mergeCell ref="V33:X33"/>
+    <mergeCell ref="Y33:AB33"/>
+    <mergeCell ref="J34:U34"/>
+    <mergeCell ref="V34:X34"/>
+    <mergeCell ref="Y34:AB34"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>